<commit_message>
labphon18 edits: analysis, figures
</commit_message>
<xml_diff>
--- a/formant_data/harmony_type.xlsx
+++ b/formant_data/harmony_type.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$60</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -520,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,7 +568,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -605,7 +608,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -725,7 +728,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -861,7 +864,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -941,7 +944,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1005,7 +1008,7 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1017,6 +1020,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B60"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>